<commit_message>
Thêm số phiếu cho Phiếu DCNB
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/PXKDCNB.xlsx
+++ b/src/main/resources/report_templates/PXKDCNB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8711FEEF-96F9-4DF0-BC4C-1A5020BB4BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA17D6-F380-416B-9FDA-6B66897BF60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>PHIẾU XUẤT KHO ĐIỀU CHUYỂN NỘI BỘ</t>
   </si>
   <si>
-    <t>Số phiếu: 005/2025_PXKDCNB</t>
-  </si>
-  <si>
     <t>Ngày: [    /     /2025]</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>${e.serialNumber}</t>
+  </si>
+  <si>
+    <t>Số phiếu:${tranCode}</t>
   </si>
 </sst>
 </file>
@@ -510,24 +510,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -536,35 +535,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,7 +917,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:G8"/>
+      <selection activeCell="B15" sqref="B15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="1"/>
@@ -939,53 +939,53 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:9" ht="27.6" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:9" ht="16.2" customHeight="1">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="17.399999999999999" customHeight="1">
+      <c r="B5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="17.399999999999999" customHeight="1">
-      <c r="B5" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="17.399999999999999" customHeight="1">
       <c r="B6" s="7"/>
@@ -996,213 +996,213 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="32" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="33" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" customHeight="1">
+      <c r="A9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A9" s="34" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" customHeight="1">
+      <c r="A10" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A10" s="34" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.8">
+      <c r="A11" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.8">
-      <c r="A11" s="31" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="8" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="31.2" customHeight="1">
+      <c r="A12" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="31.2" customHeight="1">
-      <c r="A12" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="25" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" customHeight="1">
+      <c r="A14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" customHeight="1">
-      <c r="A14" s="34" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B15" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="B15" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="11"/>
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="27.6" customHeight="1">
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:14" s="3" customFormat="1" ht="25.95" customHeight="1">
       <c r="A17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1" ht="109.8" customHeight="1">
       <c r="A18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="15" t="s">
+      <c r="F18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="8.4" customHeight="1">
       <c r="A19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+    </row>
+    <row r="20" spans="1:14" ht="21" customHeight="1">
+      <c r="A20" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-    </row>
-    <row r="20" spans="1:14" ht="21" customHeight="1">
-      <c r="A20" s="40" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:14" ht="17.399999999999999" customHeight="1">
+      <c r="A21" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-    </row>
-    <row r="21" spans="1:14" ht="17.399999999999999" customHeight="1">
-      <c r="A21" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:14" ht="18.600000000000001" customHeight="1">
       <c r="A22" s="19"/>
@@ -1215,44 +1215,44 @@
     </row>
     <row r="23" spans="1:14" ht="18.600000000000001" customHeight="1">
       <c r="A23" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="1:14" ht="18.600000000000001" customHeight="1">
+      <c r="A24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-    </row>
-    <row r="24" spans="1:14" ht="18.600000000000001" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="B24" s="26"/>
+      <c r="D24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="D24" s="6" t="s">
+    </row>
+    <row r="25" spans="1:14" ht="18.600000000000001" customHeight="1">
+      <c r="A25" s="26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="18.600000000000001" customHeight="1">
-      <c r="A25" s="41" t="s">
+      <c r="B25" s="26"/>
+      <c r="D25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="D25" s="6" t="s">
+    </row>
+    <row r="26" spans="1:14" ht="18.600000000000001" customHeight="1">
+      <c r="A26" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="18.600000000000001" customHeight="1">
-      <c r="A26" s="41" t="s">
+      <c r="B26" s="26"/>
+      <c r="D26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="D26" s="6" t="s">
+    </row>
+    <row r="27" spans="1:14" ht="18.600000000000001" customHeight="1">
+      <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="18.600000000000001" customHeight="1">
-      <c r="A27" s="41" t="s">
+      <c r="B27" s="26"/>
+      <c r="D27" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B27" s="41"/>
-      <c r="D27" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="18.600000000000001" customHeight="1">
@@ -1261,32 +1261,32 @@
     </row>
     <row r="29" spans="1:14" s="4" customFormat="1" ht="18.600000000000001" customHeight="1">
       <c r="B29" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="E29" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="F29" s="27"/>
+      <c r="G29" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" ht="18.600000000000001" customHeight="1">
       <c r="B30" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="43"/>
+        <v>40</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="28"/>
       <c r="G30" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="5" customFormat="1" ht="16.8"/>
@@ -1311,38 +1311,38 @@
     <row r="50"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B15:G16"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>